<commit_message>
fixing the data git had messed up
</commit_message>
<xml_diff>
--- a/Plots/PGcheck.xlsx
+++ b/Plots/PGcheck.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20225"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="8540" yWindow="0" windowWidth="25600" windowHeight="16620" tabRatio="500"/>
+    <workbookView xWindow="3200" yWindow="0" windowWidth="25600" windowHeight="16720" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>Pre-infection</t>
   </si>
@@ -36,13 +36,19 @@
     <t>Coverage</t>
   </si>
   <si>
-    <t>% cumulative incident cases 2025-50 in &gt;55y at baseline</t>
-  </si>
-  <si>
     <t>Observed VE in 55+</t>
   </si>
   <si>
     <t>Expected VE (ignores waning and very elderly)</t>
+  </si>
+  <si>
+    <t>average incidence rate 2025-50 in &gt;55y at baseline (/100,000/yr)</t>
+  </si>
+  <si>
+    <t>calc how much due to elderly, times ve times coverage times immunosenesce</t>
+  </si>
+  <si>
+    <t>risk of react increase- so once wane, reeinter laent so high risk of react</t>
   </si>
 </sst>
 </file>
@@ -464,10 +470,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F13"/>
+  <dimension ref="A1:F17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -477,7 +483,7 @@
     <col min="6" max="6" width="18.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="30">
+    <row r="1" spans="1:6" ht="45">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -488,13 +494,13 @@
         <v>4</v>
       </c>
       <c r="D1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>5</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:6">
@@ -508,11 +514,11 @@
         <v>30</v>
       </c>
       <c r="D2" s="5">
-        <v>78.8</v>
+        <v>160.46100000000001</v>
       </c>
       <c r="E2" s="1">
         <f>(D2/100)*(B2/100)*(C2/100)*100</f>
-        <v>9.4559999999999995</v>
+        <v>19.255320000000001</v>
       </c>
       <c r="F2" s="1"/>
     </row>
@@ -525,11 +531,11 @@
         <v>70</v>
       </c>
       <c r="D3" s="5">
-        <v>78.8</v>
+        <v>160.46100000000001</v>
       </c>
       <c r="E3" s="1">
         <f t="shared" ref="E3:E13" si="0">(D3/100)*(B3/100)*(C3/100)*100</f>
-        <v>22.063999999999997</v>
+        <v>44.929080000000006</v>
       </c>
       <c r="F3" s="1"/>
     </row>
@@ -542,11 +548,11 @@
         <v>30</v>
       </c>
       <c r="D4" s="5">
-        <v>78.8</v>
+        <v>160.46100000000001</v>
       </c>
       <c r="E4" s="1">
         <f t="shared" si="0"/>
-        <v>14.183999999999997</v>
+        <v>28.882979999999996</v>
       </c>
       <c r="F4" s="1"/>
     </row>
@@ -559,11 +565,11 @@
         <v>70</v>
       </c>
       <c r="D5" s="5">
-        <v>78.8</v>
+        <v>160.46100000000001</v>
       </c>
       <c r="E5" s="1">
         <f t="shared" si="0"/>
-        <v>33.095999999999989</v>
+        <v>67.393619999999999</v>
       </c>
       <c r="F5" s="1"/>
     </row>
@@ -576,11 +582,11 @@
         <v>30</v>
       </c>
       <c r="D6" s="5">
-        <v>78.8</v>
+        <v>160.46100000000001</v>
       </c>
       <c r="E6" s="1">
         <f t="shared" si="0"/>
-        <v>18.911999999999999</v>
+        <v>38.510640000000002</v>
       </c>
       <c r="F6" s="1"/>
     </row>
@@ -593,11 +599,11 @@
         <v>70</v>
       </c>
       <c r="D7" s="5">
-        <v>78.8</v>
+        <v>160.46100000000001</v>
       </c>
       <c r="E7" s="1">
-        <f t="shared" si="0"/>
-        <v>44.127999999999993</v>
+        <f>(D7/100)*(B7/100)*(C7/100)*100</f>
+        <v>89.858160000000012</v>
       </c>
       <c r="F7" s="1"/>
     </row>
@@ -612,11 +618,11 @@
         <v>30</v>
       </c>
       <c r="D8" s="5">
-        <v>78.8</v>
+        <v>160.46100000000001</v>
       </c>
       <c r="E8" s="1">
         <f t="shared" si="0"/>
-        <v>9.4559999999999995</v>
+        <v>19.255320000000001</v>
       </c>
       <c r="F8" s="1"/>
     </row>
@@ -629,11 +635,11 @@
         <v>70</v>
       </c>
       <c r="D9" s="5">
-        <v>78.8</v>
+        <v>160.46100000000001</v>
       </c>
       <c r="E9" s="1">
         <f t="shared" si="0"/>
-        <v>22.063999999999997</v>
+        <v>44.929080000000006</v>
       </c>
       <c r="F9" s="1"/>
     </row>
@@ -646,11 +652,11 @@
         <v>30</v>
       </c>
       <c r="D10" s="5">
-        <v>78.8</v>
+        <v>160.46100000000001</v>
       </c>
       <c r="E10" s="1">
         <f t="shared" si="0"/>
-        <v>14.183999999999997</v>
+        <v>28.882979999999996</v>
       </c>
       <c r="F10" s="1"/>
     </row>
@@ -663,11 +669,11 @@
         <v>70</v>
       </c>
       <c r="D11" s="5">
-        <v>78.8</v>
+        <v>160.46100000000001</v>
       </c>
       <c r="E11" s="1">
         <f t="shared" si="0"/>
-        <v>33.095999999999989</v>
+        <v>67.393619999999999</v>
       </c>
       <c r="F11" s="1"/>
     </row>
@@ -680,11 +686,11 @@
         <v>30</v>
       </c>
       <c r="D12" s="5">
-        <v>78.8</v>
+        <v>160.46100000000001</v>
       </c>
       <c r="E12" s="1">
         <f t="shared" si="0"/>
-        <v>18.911999999999999</v>
+        <v>38.510640000000002</v>
       </c>
       <c r="F12" s="1"/>
     </row>
@@ -697,13 +703,23 @@
         <v>70</v>
       </c>
       <c r="D13" s="5">
-        <v>78.8</v>
+        <v>160.46100000000001</v>
       </c>
       <c r="E13" s="1">
         <f t="shared" si="0"/>
-        <v>44.127999999999993</v>
+        <v>89.858160000000012</v>
       </c>
       <c r="F13" s="1"/>
+    </row>
+    <row r="16" spans="1:6">
+      <c r="D16" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="17" spans="4:4">
+      <c r="D17" t="s">
+        <v>9</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="2">

</xml_diff>

<commit_message>
- sense checks in population sizes and vaccine impact by age
</commit_message>
<xml_diff>
--- a/Plots/PGcheck.xlsx
+++ b/Plots/PGcheck.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20225"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="3200" yWindow="0" windowWidth="25600" windowHeight="16720" tabRatio="500"/>
+    <workbookView xWindow="3200" yWindow="0" windowWidth="25600" windowHeight="16740" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="13">
   <si>
     <t>Pre-infection</t>
   </si>
@@ -27,9 +27,6 @@
     <t>Post-infection</t>
   </si>
   <si>
-    <t>Vaccine</t>
-  </si>
-  <si>
     <t>VE</t>
   </si>
   <si>
@@ -49,6 +46,18 @@
   </si>
   <si>
     <t>risk of react increase- so once wane, reeinter laent so high risk of react</t>
+  </si>
+  <si>
+    <t>% disease in elderly 2025-50</t>
+  </si>
+  <si>
+    <t>vacc waning approximation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Expected VE </t>
+  </si>
+  <si>
+    <t>Mixed effects (i.e Post-infection)</t>
   </si>
 </sst>
 </file>
@@ -117,12 +126,30 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -137,10 +164,31 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="3">
+  <cellStyles count="21">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="18" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="20" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="17" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="19" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -470,37 +518,35 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F17"/>
+  <dimension ref="A1:G28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="A22" sqref="A22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="4" max="4" width="24.83203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="26.1640625" customWidth="1"/>
-    <col min="6" max="6" width="18.33203125" customWidth="1"/>
+    <col min="4" max="4" width="12.6640625" customWidth="1"/>
+    <col min="5" max="5" width="13.5" customWidth="1"/>
+    <col min="6" max="6" width="16.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="45">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:6" ht="90">
+      <c r="A1" s="1"/>
+      <c r="B1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>4</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:6">
@@ -713,18 +759,160 @@
     </row>
     <row r="16" spans="1:6">
       <c r="D16" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7">
+      <c r="D17" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="17" spans="4:4">
-      <c r="D17" t="s">
+    <row r="22" spans="1:7" ht="45">
+      <c r="A22" s="2"/>
+      <c r="B22" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D22" s="2" t="s">
         <v>9</v>
       </c>
+      <c r="E22" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="F22" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="G22" s="1"/>
+    </row>
+    <row r="23" spans="1:7">
+      <c r="A23" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B23" s="4">
+        <v>40</v>
+      </c>
+      <c r="C23" s="5">
+        <v>30</v>
+      </c>
+      <c r="D23" s="5">
+        <v>79</v>
+      </c>
+      <c r="E23" s="1">
+        <v>50</v>
+      </c>
+      <c r="F23" s="1">
+        <f t="shared" ref="F23:F28" si="1">(D23/100)*(B23/100)*(C23/100)*(E23/100)*100</f>
+        <v>4.74</v>
+      </c>
+      <c r="G23" s="1"/>
+    </row>
+    <row r="24" spans="1:7">
+      <c r="A24" s="3"/>
+      <c r="B24" s="4">
+        <v>40</v>
+      </c>
+      <c r="C24" s="5">
+        <v>70</v>
+      </c>
+      <c r="D24" s="5">
+        <v>79</v>
+      </c>
+      <c r="E24" s="1">
+        <v>50</v>
+      </c>
+      <c r="F24" s="1">
+        <f t="shared" si="1"/>
+        <v>11.060000000000002</v>
+      </c>
+      <c r="G24" s="1"/>
+    </row>
+    <row r="25" spans="1:7">
+      <c r="A25" s="3"/>
+      <c r="B25" s="4">
+        <v>60</v>
+      </c>
+      <c r="C25" s="5">
+        <v>30</v>
+      </c>
+      <c r="D25" s="5">
+        <v>79</v>
+      </c>
+      <c r="E25" s="1">
+        <v>50</v>
+      </c>
+      <c r="F25" s="1">
+        <f t="shared" si="1"/>
+        <v>7.1099999999999994</v>
+      </c>
+      <c r="G25" s="1"/>
+    </row>
+    <row r="26" spans="1:7">
+      <c r="A26" s="3"/>
+      <c r="B26" s="4">
+        <v>60</v>
+      </c>
+      <c r="C26" s="5">
+        <v>70</v>
+      </c>
+      <c r="D26" s="5">
+        <v>79</v>
+      </c>
+      <c r="E26" s="1">
+        <v>50</v>
+      </c>
+      <c r="F26" s="1">
+        <f t="shared" si="1"/>
+        <v>16.59</v>
+      </c>
+      <c r="G26" s="1"/>
+    </row>
+    <row r="27" spans="1:7">
+      <c r="A27" s="3"/>
+      <c r="B27" s="4">
+        <v>80</v>
+      </c>
+      <c r="C27" s="5">
+        <v>30</v>
+      </c>
+      <c r="D27" s="5">
+        <v>79</v>
+      </c>
+      <c r="E27" s="1">
+        <v>50</v>
+      </c>
+      <c r="F27" s="1">
+        <f t="shared" si="1"/>
+        <v>9.48</v>
+      </c>
+      <c r="G27" s="1"/>
+    </row>
+    <row r="28" spans="1:7">
+      <c r="A28" s="3"/>
+      <c r="B28" s="4">
+        <v>80</v>
+      </c>
+      <c r="C28" s="5">
+        <v>70</v>
+      </c>
+      <c r="D28" s="5">
+        <v>79</v>
+      </c>
+      <c r="E28" s="1">
+        <v>50</v>
+      </c>
+      <c r="F28" s="1">
+        <f t="shared" si="1"/>
+        <v>22.120000000000005</v>
+      </c>
+      <c r="G28" s="1"/>
     </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="3">
     <mergeCell ref="A2:A7"/>
     <mergeCell ref="A8:A13"/>
+    <mergeCell ref="A23:A28"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>

</xml_diff>